<commit_message>
updated test cases in signup page
</commit_message>
<xml_diff>
--- a/07_Testing/signup.xlsx
+++ b/07_Testing/signup.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="141">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -262,7 +262,7 @@
     <t>TC23</t>
   </si>
   <si>
-    <t>Check the ""Sign In"" button functionality for already signed-up users.</t>
+    <t>Check the ""Sign in"" button functionality for already signed-up users.</t>
   </si>
   <si>
     <t>Click the "Sign In" button and ensure it redirects to the sign-in page.</t>
@@ -341,6 +341,99 @@
   </si>
   <si>
     <t>System can handle high traffic without significant performance degradation.</t>
+  </si>
+  <si>
+    <t>TC30</t>
+  </si>
+  <si>
+    <t>Verify compatibility with major browsers.</t>
+  </si>
+  <si>
+    <t>Open the signup page in different browsers such as Google Chrome, Mozilla Firefox, Microsoft Edge, Safari, and Opera. Ensure all elements are displayed correctly, and functionality remains consistent across browsers.</t>
+  </si>
+  <si>
+    <t>All elements are displayed correctly and functionality remains consistent across major browsers.</t>
+  </si>
+  <si>
+    <t>TC31</t>
+  </si>
+  <si>
+    <t>Check responsiveness across browsers.</t>
+  </si>
+  <si>
+    <t>Test the signup page on different browsers across various devices (desktop, tablet, smartphone). Ensure the layout and functionality adapt well to different screen sizes and resolutions.</t>
+  </si>
+  <si>
+    <t>Layout and functionality adapt well to different screen sizes and resolutions across different browsers.</t>
+  </si>
+  <si>
+    <t>TC32</t>
+  </si>
+  <si>
+    <t>Load Testing.</t>
+  </si>
+  <si>
+    <t>Simulate a large number of concurrent users accessing the signup page simultaneously.</t>
+  </si>
+  <si>
+    <t>The system can handle a large number of concurrent users without crashing or significantly slowing down.</t>
+  </si>
+  <si>
+    <t>TC33</t>
+  </si>
+  <si>
+    <t>Scalability Testing.</t>
+  </si>
+  <si>
+    <t>Gradually increase the number of users accessing the signup page to test the system's ability to scale.</t>
+  </si>
+  <si>
+    <t>The system scales seamlessly with increased user load.</t>
+  </si>
+  <si>
+    <t>TC34</t>
+  </si>
+  <si>
+    <t>Response Time and Throughput.</t>
+  </si>
+  <si>
+    <t>Measure the time taken for the server to respond and the number of transactions processed per unit time under normal conditions.</t>
+  </si>
+  <si>
+    <t>Server response time is within acceptable limits</t>
+  </si>
+  <si>
+    <t>and the system processes transactions efficiently.</t>
+  </si>
+  <si>
+    <t>Stress Testing.</t>
+  </si>
+  <si>
+    <t>Apply a load beyond the system's capacity to verify its behavior under stress.</t>
+  </si>
+  <si>
+    <t>The system remains stable and responsive even under stress</t>
+  </si>
+  <si>
+    <t>with graceful degradation if necessary.</t>
+  </si>
+  <si>
+    <t>TC35</t>
+  </si>
+  <si>
+    <t>TC36</t>
+  </si>
+  <si>
+    <t>Resource Utilization and Efficiency.</t>
+  </si>
+  <si>
+    <t>Monitor system resources (CPU, memory, disk I/O) during peak usage to ensure efficient resource utilization.</t>
+  </si>
+  <si>
+    <t>System resources are optimally utilized</t>
+  </si>
+  <si>
+    <t>and performance remains stable even during peak usage.</t>
   </si>
 </sst>
 </file>
@@ -374,13 +467,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -1020,18 +1114,40 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
+    <row r="28">
+      <c r="A28" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
     <row r="29">
       <c r="A29" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>11</v>
@@ -1044,16 +1160,16 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>11</v>
@@ -1066,16 +1182,16 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>11</v>
@@ -1088,25 +1204,186 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+        <v>113</v>
+      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>